<commit_message>
New cleaning -staff data
</commit_message>
<xml_diff>
--- a/Data Cleaning(with pandas) Start1.xlsx
+++ b/Data Cleaning(with pandas) Start1.xlsx
@@ -8,19 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OJ 001\Desktop\DataScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57D061B-7FFB-419A-8D67-D7BFDF65A32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D6B4DD-8B2E-4BE1-BFA3-7B5C96DBA0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot Table" sheetId="2" r:id="rId1"/>
+    <sheet name="Sales" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Sales">Sales!$B$9</definedName>
+    <definedName name="Slicer_Department">#N/A</definedName>
+    <definedName name="Slicer_Region">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="41" r:id="rId3"/>
+  </pivotCaches>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId4"/>
+        <x14:slicerCache r:id="rId5"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -251,6 +271,21 @@
   </si>
   <si>
     <t xml:space="preserve">CISCO SYSTEMS INC. </t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Revenue</t>
+  </si>
+  <si>
+    <t>Sum of Profit Margin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -258,7 +293,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -312,9 +347,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -324,30 +357,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -358,6 +423,709 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Department">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6FAC387-33FA-1A56-885C-8418A60D5099}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Department"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4184650" y="196850"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Region">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B495267E-8EE7-3ED4-2D4E-05D54AC87AF9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Region"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6464300" y="177800"/>
+              <a:ext cx="1828800" cy="2505075"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="OJ 001" refreshedDate="45768.78577800926" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{FA7D546F-56CD-4EC6-A37A-46D1E8B58E94}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-05-30T00:00:00" maxDate="2023-06-03T00:00:00"/>
+    </cacheField>
+    <cacheField name="Client" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Contact" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Department" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Cloud Tech"/>
+        <s v="Strategy"/>
+        <s v="Operations"/>
+        <s v="Big Data"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Texas"/>
+        <s v="New York"/>
+        <s v="Florida"/>
+        <s v="California"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Payment" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Revenue" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="7500"/>
+    </cacheField>
+    <cacheField name="Profit Margin" numFmtId="10">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="8.9180327868852466E-2" maxValue="0.53815789473684206" count="27">
+        <n v="0.13288888888888889"/>
+        <n v="0.27500000000000002"/>
+        <n v="0.2717845117845118"/>
+        <s v="N/A"/>
+        <n v="0.1368"/>
+        <n v="8.9180327868852466E-2"/>
+        <n v="0.14486486486486491"/>
+        <n v="0.53815789473684206"/>
+        <n v="0.43444444444444452"/>
+        <n v="0.23921568627450979"/>
+        <n v="0.30210526315789471"/>
+        <n v="0.16633333333333331"/>
+        <n v="0.17333333333333331"/>
+        <n v="0.32915824915824909"/>
+        <n v="0.21515151515151509"/>
+        <n v="0.17052631578947369"/>
+        <n v="0.12745901639344259"/>
+        <n v="0.12874692874692881"/>
+        <n v="0.16044444444444439"/>
+        <n v="0.21199999999999999"/>
+        <n v="0.25695238095238088"/>
+        <n v="0.19815384615384621"/>
+        <n v="0.22186666666666671"/>
+        <n v="0.24"/>
+        <n v="0.2164324324324324"/>
+        <n v="0.21333333333333329"/>
+        <n v="0.1"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="2072352352"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="28">
+  <r>
+    <d v="2023-05-30T00:00:00"/>
+    <s v="AMAZON.COM INC. "/>
+    <s v="Bill Smith"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Transfer"/>
+    <n v="4500"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2023-05-30T00:00:00"/>
+    <s v="TESLA INC. "/>
+    <s v="Ken Singh"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="PayPal"/>
+    <n v="3800"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2023-05-30T00:00:00"/>
+    <s v="NETFLIX INC. "/>
+    <s v="Harley Fritz"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N/A"/>
+    <n v="3712.5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2023-05-30T00:00:00"/>
+    <s v="THE PROCTER &amp; GAMBLE COMPANY "/>
+    <s v="Nyla Novak"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="N/A"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-05-30T00:00:00"/>
+    <s v="THE GOLDMAN SACHS GROUP INC. "/>
+    <s v="David Rasmussen"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="Check"/>
+    <n v="5000"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="JPMORGAN CHASE &amp; CO. "/>
+    <s v="Ivan Hiney"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Transfer"/>
+    <n v="6100"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="MORGAN STANLEY "/>
+    <s v="Jonha Ma"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Transfer"/>
+    <n v="4625"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="CITIGROUP INC. "/>
+    <s v="Jordan Boone"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Transfer"/>
+    <n v="3800"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="BANK OF AMERICA CORPORATION "/>
+    <s v="Kylee Townsend"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Card"/>
+    <n v="3600"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="WALMART INC. "/>
+    <s v="Nora Rollins"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Check"/>
+    <n v="5100"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="TARGET CORPORATION "/>
+    <s v="Brendan Wallace"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Check"/>
+    <n v="4750"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="COSTCO WHOLESALE CORPORATION "/>
+    <s v="Conor Wise"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="Transfer"/>
+    <n v="6000"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <d v="2023-05-31T00:00:00"/>
+    <s v="MCDONALD'S CORPORATION "/>
+    <s v="Steven Michael"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Check"/>
+    <n v="4500"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="EXXON MOBIL CORPORATION "/>
+    <s v="Lucia Mckay"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Card"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="VERIZON COMMUNICATIONS INC. "/>
+    <s v="Jose Roach"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Transfer"/>
+    <n v="3712.5"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="THE HOME DEPOT INC. "/>
+    <s v="Franklin Wrigt"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Transfer"/>
+    <n v="4950"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="CISCO SYSTEMS INC. "/>
+    <s v="Alia Thornton"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="Transfer"/>
+    <n v="4750"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="CHEVRON CORPORATION "/>
+    <s v="Denzel Flores"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="Transfer"/>
+    <n v="7320"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="AT&amp;T INC. "/>
+    <s v="Bruno Cordova"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Transfer"/>
+    <n v="5087.5"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="INTEL CORPORATION "/>
+    <s v="Jaylynn Napp"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Transfer"/>
+    <n v="4500"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <d v="2023-06-01T00:00:00"/>
+    <s v="GENERAL MOTORS COMPANY "/>
+    <s v="Bruce Rich"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Card"/>
+    <n v="4250"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <d v="2023-06-02T00:00:00"/>
+    <s v="MICROSOFT CORPORATION "/>
+    <s v="Arturo Moore"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="PayPal"/>
+    <n v="5250"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <d v="2023-06-02T00:00:00"/>
+    <s v="COMCAST CORPORATION "/>
+    <s v="Bryce Carpenter"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="PayPal"/>
+    <n v="6500"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <d v="2023-06-02T00:00:00"/>
+    <s v="DELL TECHNOLOGIES INC. "/>
+    <s v="Jaidyn Andersen"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="PayPal"/>
+    <n v="7500"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <d v="2023-06-02T00:00:00"/>
+    <s v="JOHNSON &amp; JOHNSON "/>
+    <s v="Mark Walm"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Transfer"/>
+    <n v="5500"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <d v="2023-06-02T00:00:00"/>
+    <s v="FEDEX CORPORATION "/>
+    <s v="Harry Lee"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Transfer"/>
+    <n v="4625"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <d v="2023-06-02T00:00:00"/>
+    <s v="GENERAL ELECTRIC COMPANY "/>
+    <s v="Josh Johnson"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Transfer"/>
+    <n v="4500"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <d v="2023-06-02T00:00:00"/>
+    <s v="LOCKHEED MARTIN CORPORATION "/>
+    <s v="Mik Naam"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Card"/>
+    <n v="5400"/>
+    <x v="26"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5484AC0B-98D8-449A-98F4-4AD107499E3B}" name="PivotTable6" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+  <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="28">
+        <item x="5"/>
+        <item x="26"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="18"/>
+        <item x="11"/>
+        <item x="15"/>
+        <item x="12"/>
+        <item x="21"/>
+        <item x="19"/>
+        <item x="25"/>
+        <item x="14"/>
+        <item x="24"/>
+        <item x="22"/>
+        <item x="9"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="13"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Revenue" fld="6" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Sum of Profit Margin" fld="7" baseField="3" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Department" xr10:uid="{93D70268-9EB4-4415-BD73-3155529D8AE9}" sourceName="Department">
+  <pivotTables>
+    <pivotTable tabId="2" name="PivotTable6"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="2072352352">
+      <items count="4">
+        <i x="3" s="1"/>
+        <i x="0" s="1"/>
+        <i x="2" s="1"/>
+        <i x="1" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Region" xr10:uid="{5BB45842-FBE4-46D1-B7C1-C4FCF5EBEDE5}" sourceName="Region">
+  <pivotTables>
+    <pivotTable tabId="2" name="PivotTable6"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="2072352352">
+      <items count="4">
+        <i x="3" s="1"/>
+        <i x="2" s="1"/>
+        <i x="1" s="1"/>
+        <i x="0" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Department" xr10:uid="{E4FCA833-1478-48F5-A0C0-0E7EEC42BDAA}" cache="Slicer_Department" caption="Department" rowHeight="241300"/>
+  <slicer name="Region" xr10:uid="{2564273B-7374-459B-9F66-D79F9D360D18}" cache="Slicer_Region" caption="Region" rowHeight="241300"/>
+</slicers>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C19952C8-2B30-43A7-8A44-7EB8E64E5250}" name="Table1" displayName="Table1" ref="A1:H29" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:H29" xr:uid="{C19952C8-2B30-43A7-8A44-7EB8E64E5250}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9491DA09-F32C-4590-AA93-B19E17F57ECA}" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4078C0EF-1A9E-405F-8225-BD69C9AAE85F}" name="Client"/>
+    <tableColumn id="3" xr3:uid="{4FE45419-8861-4BF1-8A70-06CAE3134A75}" name="Contact"/>
+    <tableColumn id="4" xr3:uid="{7F9999C8-4945-4886-BB65-3A4593D32393}" name="Department"/>
+    <tableColumn id="5" xr3:uid="{40C98D67-DEB6-437F-8AFF-46816689164A}" name="Region"/>
+    <tableColumn id="6" xr3:uid="{50A71D0B-FB1B-4B57-8DCC-C454125958D0}" name="Payment"/>
+    <tableColumn id="7" xr3:uid="{D20536B8-1AD7-4FE9-AEF1-44DA21D051C9}" name="Revenue" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{597A03FE-E274-4313-9B35-8AE5CD2148CB}" name="Profit Margin" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -644,56 +1412,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05C0F99-DF0B-4939-93FE-39C752A548AA}">
+  <dimension ref="A3:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="4">
+        <v>32250</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1.4757868517868515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="4">
+        <v>32250</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1.4757868517868515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>32475</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1.8808573702362974</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>32475</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1.8808573702362974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4">
+        <v>23070</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.6011186655162496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4">
+        <v>23070</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.6011186655162496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
+        <v>41537.5</v>
+      </c>
+      <c r="C10" s="13">
+        <v>1.7365707903707908</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4">
+        <v>41537.5</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1.7365707903707908</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="4">
+        <v>129332.5</v>
+      </c>
+      <c r="C12" s="13">
+        <v>5.6943336779101896</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" customWidth="1"/>
     <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10" style="4" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
         <v>45076</v>
       </c>
       <c r="B2" t="s">
@@ -711,18 +1619,15 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="4">
         <v>4500</v>
       </c>
-      <c r="H2" s="7">
-        <v>4500</v>
-      </c>
-      <c r="I2" s="5">
+      <c r="H2" s="3">
         <v>0.13288888888888889</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="9">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
         <v>45076</v>
       </c>
       <c r="B3" t="s">
@@ -740,18 +1645,15 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="4">
         <v>3800</v>
       </c>
-      <c r="H3" s="7">
-        <v>3800</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="H3" s="3">
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
         <v>45076</v>
       </c>
       <c r="B4" t="s">
@@ -769,18 +1671,15 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="4">
         <v>3712.5</v>
       </c>
-      <c r="H4" s="7">
-        <v>3712.5</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="H4" s="3">
         <v>0.2717845117845118</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="9">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
         <v>45076</v>
       </c>
       <c r="B5" t="s">
@@ -798,18 +1697,15 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>0</v>
       </c>
-      <c r="H5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="9">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
         <v>45076</v>
       </c>
       <c r="B6" t="s">
@@ -827,18 +1723,15 @@
       <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="4">
         <v>5000</v>
       </c>
-      <c r="H6" s="7">
-        <v>5000</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="3">
         <v>0.1368</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="9">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>45077</v>
       </c>
       <c r="B7" t="s">
@@ -856,18 +1749,15 @@
       <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>6100</v>
       </c>
-      <c r="H7" s="7">
-        <v>6100</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="H7" s="3">
         <v>8.9180327868852466E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
         <v>45077</v>
       </c>
       <c r="B8" t="s">
@@ -885,18 +1775,15 @@
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="4">
         <v>4625</v>
       </c>
-      <c r="H8" s="7">
-        <v>4625</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="H8" s="3">
         <v>0.14486486486486491</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>45077</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -914,18 +1801,15 @@
       <c r="F9" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <v>3800</v>
       </c>
-      <c r="H9" s="7">
-        <v>3800</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="H9" s="3">
         <v>0.53815789473684206</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
         <v>45077</v>
       </c>
       <c r="B10" t="s">
@@ -943,18 +1827,15 @@
       <c r="F10" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="4">
         <v>3600</v>
       </c>
-      <c r="H10" s="7">
-        <v>3600</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="H10" s="3">
         <v>0.43444444444444452</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="9">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
         <v>45077</v>
       </c>
       <c r="B11" t="s">
@@ -972,18 +1853,15 @@
       <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <v>5100</v>
       </c>
-      <c r="H11" s="7">
-        <v>5100</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="H11" s="3">
         <v>0.23921568627450979</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
         <v>45077</v>
       </c>
       <c r="B12" t="s">
@@ -1001,18 +1879,15 @@
       <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <v>4750</v>
       </c>
-      <c r="H12" s="7">
-        <v>4750</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="H12" s="3">
         <v>0.30210526315789471</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
         <v>45077</v>
       </c>
       <c r="B13" t="s">
@@ -1030,18 +1905,15 @@
       <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="4">
         <v>6000</v>
       </c>
-      <c r="H13" s="7">
-        <v>6000</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="H13" s="3">
         <v>0.16633333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
         <v>45077</v>
       </c>
       <c r="B14" t="s">
@@ -1059,18 +1931,15 @@
       <c r="F14" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="4">
         <v>4500</v>
       </c>
-      <c r="H14" s="7">
-        <v>4500</v>
-      </c>
-      <c r="I14" s="5">
+      <c r="H14" s="3">
         <v>0.17333333333333331</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
         <v>45078</v>
       </c>
       <c r="B15" t="s">
@@ -1088,18 +1957,15 @@
       <c r="F15" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4">
         <v>0</v>
       </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5" t="s">
+      <c r="H15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
         <v>45078</v>
       </c>
       <c r="B16" t="s">
@@ -1117,18 +1983,15 @@
       <c r="F16" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="4">
         <v>3712.5</v>
       </c>
-      <c r="H16" s="7">
-        <v>3712.5</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="H16" s="3">
         <v>0.32915824915824909</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
         <v>45078</v>
       </c>
       <c r="B17" t="s">
@@ -1146,18 +2009,15 @@
       <c r="F17" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4">
         <v>4950</v>
       </c>
-      <c r="H17" s="7">
-        <v>4950</v>
-      </c>
-      <c r="I17" s="5">
+      <c r="H17" s="3">
         <v>0.21515151515151509</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="9">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
         <v>45078</v>
       </c>
       <c r="B18" t="s">
@@ -1175,18 +2035,15 @@
       <c r="F18" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="4">
         <v>4750</v>
       </c>
-      <c r="H18" s="7">
-        <v>4750</v>
-      </c>
-      <c r="I18" s="5">
+      <c r="H18" s="3">
         <v>0.17052631578947369</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="9">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
         <v>45078</v>
       </c>
       <c r="B19" t="s">
@@ -1204,18 +2061,15 @@
       <c r="F19" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="4">
         <v>7320</v>
       </c>
-      <c r="H19" s="7">
-        <v>7320</v>
-      </c>
-      <c r="I19" s="5">
+      <c r="H19" s="3">
         <v>0.12745901639344259</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="9">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
         <v>45078</v>
       </c>
       <c r="B20" t="s">
@@ -1233,18 +2087,15 @@
       <c r="F20" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="4">
         <v>5087.5</v>
       </c>
-      <c r="H20" s="7">
-        <v>5087.5</v>
-      </c>
-      <c r="I20" s="5">
+      <c r="H20" s="3">
         <v>0.12874692874692881</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="9">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
         <v>45078</v>
       </c>
       <c r="B21" t="s">
@@ -1262,18 +2113,15 @@
       <c r="F21" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="4">
         <v>4500</v>
       </c>
-      <c r="H21" s="7">
-        <v>4500</v>
-      </c>
-      <c r="I21" s="5">
+      <c r="H21" s="3">
         <v>0.16044444444444439</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="9">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
         <v>45078</v>
       </c>
       <c r="B22" t="s">
@@ -1291,18 +2139,15 @@
       <c r="F22" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="4">
         <v>4250</v>
       </c>
-      <c r="H22" s="7">
-        <v>4250</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="H22" s="3">
         <v>0.21199999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="9">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
         <v>45079</v>
       </c>
       <c r="B23" t="s">
@@ -1320,18 +2165,15 @@
       <c r="F23" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="4">
         <v>5250</v>
       </c>
-      <c r="H23" s="7">
-        <v>5250</v>
-      </c>
-      <c r="I23" s="5">
+      <c r="H23" s="3">
         <v>0.25695238095238088</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="9">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
         <v>45079</v>
       </c>
       <c r="B24" t="s">
@@ -1349,18 +2191,15 @@
       <c r="F24" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="4">
         <v>6500</v>
       </c>
-      <c r="H24" s="7">
-        <v>6500</v>
-      </c>
-      <c r="I24" s="5">
+      <c r="H24" s="3">
         <v>0.19815384615384621</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="9">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
         <v>45079</v>
       </c>
       <c r="B25" t="s">
@@ -1378,18 +2217,15 @@
       <c r="F25" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="4">
         <v>7500</v>
       </c>
-      <c r="H25" s="7">
-        <v>7500</v>
-      </c>
-      <c r="I25" s="5">
+      <c r="H25" s="3">
         <v>0.22186666666666671</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="9">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="5">
         <v>45079</v>
       </c>
       <c r="B26" t="s">
@@ -1407,18 +2243,15 @@
       <c r="F26" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="4">
         <v>5500</v>
       </c>
-      <c r="H26" s="7">
-        <v>5500</v>
-      </c>
-      <c r="I26" s="5">
+      <c r="H26" s="3">
         <v>0.24</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="9">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
         <v>45079</v>
       </c>
       <c r="B27" t="s">
@@ -1436,18 +2269,15 @@
       <c r="F27" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="4">
         <v>4625</v>
       </c>
-      <c r="H27" s="7">
-        <v>4625</v>
-      </c>
-      <c r="I27" s="5">
+      <c r="H27" s="3">
         <v>0.2164324324324324</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="9">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
         <v>45079</v>
       </c>
       <c r="B28" t="s">
@@ -1465,18 +2295,15 @@
       <c r="F28" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="4">
         <v>4500</v>
       </c>
-      <c r="H28" s="7">
-        <v>4500</v>
-      </c>
-      <c r="I28" s="5">
+      <c r="H28" s="3">
         <v>0.21333333333333329</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="9">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="5">
         <v>45079</v>
       </c>
       <c r="B29" t="s">
@@ -1494,17 +2321,17 @@
       <c r="F29" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="4">
         <v>5400</v>
       </c>
-      <c r="H29" s="7">
-        <v>5400</v>
-      </c>
-      <c r="I29" s="5">
+      <c r="H29" s="3">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>